<commit_message>
Save worksheet extensions for all DataBar-styled conditional formats, not only for having more than one color, to correctly process min/max values
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/ConditionalFormatting/CFDataBar.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/ConditionalFormatting/CFDataBar.xlsx
@@ -359,7 +359,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<x:worksheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
@@ -397,6 +397,11 @@
         <x:cfvo type="percent" val="100"/>
         <x:color rgb="FFFF0000"/>
       </x:dataBar>
+      <x:extLst>
+        <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{0cf7a109-a037-492e-9fee-4b588b6e219c}</x14:id>
+        </x:ext>
+      </x:extLst>
     </x:cfRule>
   </x:conditionalFormatting>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
@@ -404,5 +409,26 @@
   <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
   <x:headerFooter/>
   <x:tableParts count="0"/>
+  <x:extLst>
+    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{0cf7a109-a037-492e-9fee-4b588b6e219c}">
+            <x14:dataBar minLength="0" maxLength="100" showValue="0" gradient="1">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>100</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>A1:A4</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </x:ext>
+  </x:extLst>
 </x:worksheet>
 </file>
</xml_diff>